<commit_message>
se añade formato de cotizacion
</commit_message>
<xml_diff>
--- a/Request.xlsx
+++ b/Request.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacod\Desktop\FylsaERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cocoy\Documents\Projects\Fylsa\FylsaERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464380AD-AFD5-4937-ADC0-0810C3FF989F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562DE094-FA80-44BB-97ED-8ADF2AD507BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{2202F2AB-1EFC-4DF0-896B-A19C38AB749D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6948" xr2:uid="{2202F2AB-1EFC-4DF0-896B-A19C38AB749D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t xml:space="preserve">Metodos </t>
   </si>
@@ -239,6 +239,36 @@
   </si>
   <si>
     <t>"URL"</t>
+  </si>
+  <si>
+    <t>{
+    "DATE": "18/03/15",
+    "COMPANY": "BARCEL",
+    "ADDRESSED": "Ingeniero Juan Carlos",
+    "REASON": "Suministro de Material Electrico",
+    "COST": 2000,
+    "DELIVERY_TIME": "3 SEMANAS",
+    "PAYMENT_CONDITIONS": "28 dias",
+    "COTIZACION_SERVICE": [
+        {
+            "ITEM": 1,
+            "DESCIPTION": "codo conduit 2 pulgadas",
+            "PROVIDE": "Suministro",
+            "CANTITY": 2,
+            "MEASURE_UNIT": "PZA",
+            "SALE_PRICE": 200
+        },
+        {
+            "ITEM": 2,
+            "DESCIPTION": "Cable pulgada 2 ",
+            "PROVIDE": "Suministro e instalacion",
+            "CANTITY": 10,
+            "MEASURE_UNIT": "MT",
+            "SALE_PRICE": 100
+        }
+    ],
+    "USER_ID": 1
+}</t>
   </si>
 </sst>
 </file>
@@ -663,28 +693,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125BFC7E-081B-4FC7-A42F-E8286AF1EDC7}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="52.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -698,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -712,12 +742,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -731,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -745,12 +775,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -767,7 +797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -781,7 +811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -795,7 +825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
@@ -809,7 +839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -823,12 +853,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -842,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -856,7 +886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
@@ -870,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -885,7 +915,7 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -899,12 +929,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -918,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
@@ -932,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -940,13 +970,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Se implemento el metodo para el Login, Tambien se creo el metodo para buscar producto
</commit_message>
<xml_diff>
--- a/Request.xlsx
+++ b/Request.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cocoy\Documents\Projects\Fylsa\FylsaERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacod\Desktop\FylsaERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562DE094-FA80-44BB-97ED-8ADF2AD507BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD57E78-6331-4320-AE47-CAA79AF0017B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6948" xr2:uid="{2202F2AB-1EFC-4DF0-896B-A19C38AB749D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{2202F2AB-1EFC-4DF0-896B-A19C38AB749D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t xml:space="preserve">Metodos </t>
   </si>
@@ -269,6 +269,19 @@
     ],
     "USER_ID": 1
 }</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/products/find</t>
+  </si>
+  <si>
+    <t>desc= "Descripcion del Producto"</t>
+  </si>
+  <si>
+    <t>[{
+    "NAME": "BARCEL",
+    "DIRECTION": "IZCALLI CUAUHTEMOC 3",
+    "RFC": "JUNA96020"
+}  ]</t>
   </si>
 </sst>
 </file>
@@ -691,30 +704,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125BFC7E-081B-4FC7-A42F-E8286AF1EDC7}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" customWidth="1"/>
-    <col min="4" max="4" width="52.5546875" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -728,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -742,12 +755,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -761,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -775,236 +788,251 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="17" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" xr:uid="{7F053010-2E65-4818-9117-B5E6E18769E1}"/>
-    <hyperlink ref="A11" r:id="rId2" xr:uid="{DE995AFB-7C92-4D41-9DA3-615A507B7322}"/>
-    <hyperlink ref="A12" r:id="rId3" xr:uid="{C120884D-70CD-4DEC-9E73-3B9B325D0EF2}"/>
-    <hyperlink ref="A13" r:id="rId4" xr:uid="{6D039909-22CC-478D-96A6-C35483603886}"/>
-    <hyperlink ref="A16" r:id="rId5" xr:uid="{A7650FA1-5B59-40CB-9A3E-A06A5942332B}"/>
-    <hyperlink ref="A17" r:id="rId6" xr:uid="{B1E06D82-8814-44EA-9B3C-ACC474FC51B4}"/>
-    <hyperlink ref="A18" r:id="rId7" xr:uid="{538FEE5C-D96F-42D9-B5CC-37CDD81BFDBA}"/>
-    <hyperlink ref="A19" r:id="rId8" xr:uid="{7EB599B6-4828-41E5-981A-8CEE0A044BC3}"/>
-    <hyperlink ref="A22" r:id="rId9" xr:uid="{B180247C-1837-4F42-BF6F-4749DB010C86}"/>
-    <hyperlink ref="A23" r:id="rId10" xr:uid="{9A00D0BD-BFFF-4985-B8C8-7A58982729FA}"/>
-    <hyperlink ref="A24" r:id="rId11" xr:uid="{929A31FE-53EB-4B91-A2B4-ABD5C6A2965D}"/>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{7F053010-2E65-4818-9117-B5E6E18769E1}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{DE995AFB-7C92-4D41-9DA3-615A507B7322}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{C120884D-70CD-4DEC-9E73-3B9B325D0EF2}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{6D039909-22CC-478D-96A6-C35483603886}"/>
+    <hyperlink ref="A17" r:id="rId5" xr:uid="{A7650FA1-5B59-40CB-9A3E-A06A5942332B}"/>
+    <hyperlink ref="A18" r:id="rId6" xr:uid="{B1E06D82-8814-44EA-9B3C-ACC474FC51B4}"/>
+    <hyperlink ref="A19" r:id="rId7" xr:uid="{538FEE5C-D96F-42D9-B5CC-37CDD81BFDBA}"/>
+    <hyperlink ref="A20" r:id="rId8" xr:uid="{7EB599B6-4828-41E5-981A-8CEE0A044BC3}"/>
+    <hyperlink ref="A23" r:id="rId9" xr:uid="{B180247C-1837-4F42-BF6F-4749DB010C86}"/>
+    <hyperlink ref="A24" r:id="rId10" xr:uid="{9A00D0BD-BFFF-4985-B8C8-7A58982729FA}"/>
+    <hyperlink ref="A25" r:id="rId11" xr:uid="{929A31FE-53EB-4B91-A2B4-ABD5C6A2965D}"/>
+    <hyperlink ref="A8" r:id="rId12" xr:uid="{5915EE82-4FFA-461D-B242-0EDFCA646946}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>